<commit_message>
added excel tabels from Eurostat
</commit_message>
<xml_diff>
--- a/figures/worldmap/airports.xlsx
+++ b/figures/worldmap/airports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barend/Desktop/Thesis/demandmap/figures/worldmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45586DA-9AE8-1C49-BCCB-85688A649F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D511BC-3C43-184C-AA5A-8E74E485F3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Airports" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2693" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2695" uniqueCount="592">
   <si>
     <t>51.4775, -0.461389</t>
   </si>
@@ -1805,6 +1805,12 @@
   </si>
   <si>
     <t>MAPUTO airport</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -1910,7 +1916,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -2256,11 +2262,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2331,6 +2374,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2915,10 +2964,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U21"/>
+  <dimension ref="A1:W21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView zoomScale="68" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="Z9" sqref="Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2927,7 +2976,7 @@
     <col min="2" max="21" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11"/>
       <c r="B1" s="15" t="s">
         <v>26</v>
@@ -2989,8 +3038,11 @@
       <c r="U1" s="13" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W1" s="38" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>26</v>
       </c>
@@ -3074,8 +3126,11 @@
         <f>IFERROR(VLOOKUP(U$1,Tabelle2!$AQ:$AR,2,FALSE),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W2" s="39">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>35</v>
       </c>
@@ -3159,8 +3214,11 @@
         <f>IFERROR(VLOOKUP(U$1,Tabelle2!$G:$H,2,FALSE),0)</f>
         <v>488</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W3" s="40">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>29</v>
       </c>
@@ -3244,8 +3302,11 @@
         <f>IFERROR(VLOOKUP(U$1,Tabelle2!$J:$K,2,FALSE),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W4" s="40">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>30</v>
       </c>
@@ -3329,8 +3390,11 @@
         <f>IFERROR(VLOOKUP(U$1,Tabelle2!$AH:$AI,2,FALSE),0)</f>
         <v>1255</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W5" s="40">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>32</v>
       </c>
@@ -3411,8 +3475,11 @@
         <v>1130</v>
       </c>
       <c r="U6" s="31"/>
-    </row>
-    <row r="7" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W6" s="40">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>25</v>
       </c>
@@ -3496,8 +3563,11 @@
         <f>IFERROR(VLOOKUP(U$1,Tabelle2!A:B,2,FALSE),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W7" s="40">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>33</v>
       </c>
@@ -3581,8 +3651,11 @@
         <f>IFERROR(VLOOKUP(U$1,Tabelle2!$Y:$HZ,2,FALSE),0)</f>
         <v>3100</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W8" s="40">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>40</v>
       </c>
@@ -3666,8 +3739,11 @@
         <f>IFERROR(VLOOKUP(U$1,Tabelle2!$AW:$AX,2,FALSE),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W9" s="40">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>38</v>
       </c>
@@ -3751,8 +3827,11 @@
         <f>IFERROR(VLOOKUP(U$1,Tabelle2!$AE:$AF,2,FALSE),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W10" s="40">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>27</v>
       </c>
@@ -3835,8 +3914,11 @@
         <f>IFERROR(VLOOKUP(U$1,Tabelle2!$D:$E,2,FALSE),0)</f>
         <v/>
       </c>
-    </row>
-    <row r="12" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W11" s="40">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>255</v>
       </c>
@@ -3898,8 +3980,11 @@
       <c r="U12" s="31">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W12" s="40" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>36</v>
       </c>
@@ -3983,8 +4068,11 @@
         <f>IFERROR(VLOOKUP(U$1,Tabelle2!$BC:$BD,2,FALSE),0)</f>
         <v>2642</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W13" s="40">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>37</v>
       </c>
@@ -4068,8 +4156,11 @@
         <f>IFERROR(VLOOKUP(U$1,Tabelle2!$P:$Q,2,FALSE),0)</f>
         <v>5504</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W14" s="40">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>231</v>
       </c>
@@ -4153,8 +4244,11 @@
         <f>IFERROR(VLOOKUP(U$1,Tabelle2!$M:$N,2,FALSE),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W15" s="40">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>34</v>
       </c>
@@ -4238,8 +4332,11 @@
         <f>IFERROR(VLOOKUP(U$1,Tabelle2!$AB:$AC,2,FALSE),0)</f>
         <v>2943</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W16" s="40">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>28</v>
       </c>
@@ -4323,8 +4420,11 @@
         <f>IFERROR(VLOOKUP(U$1,Tabelle2!$AK:$AL,2,FALSE),0)</f>
         <v>1561</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W17" s="40">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>31</v>
       </c>
@@ -4408,8 +4508,11 @@
         <f>IFERROR(VLOOKUP(U$1,Tabelle2!$AN:$AO,2,FALSE),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W18" s="40">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>39</v>
       </c>
@@ -4493,8 +4596,11 @@
         <f>IFERROR(VLOOKUP(U$1,Tabelle2!$S:$T,2,FALSE),0)</f>
         <v>1161</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W19" s="40">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>41</v>
       </c>
@@ -4578,8 +4684,11 @@
         <f>IFERROR(VLOOKUP(U$1,Tabelle2!$AT:$AU,2,FALSE),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W20" s="40">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>264</v>
       </c>
@@ -4662,6 +4771,9 @@
       <c r="U21" s="24">
         <f>IFERROR(VLOOKUP(U$1,Tabelle2!$AZ:$BA,2,FALSE),0)</f>
         <v>0</v>
+      </c>
+      <c r="W21" s="41">
+        <v>2019</v>
       </c>
     </row>
   </sheetData>
@@ -4673,13 +4785,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BD222"/>
   <sheetViews>
-    <sheetView topLeftCell="AF1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="BC2" sqref="BC2:BC98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
     <col min="4" max="4" width="21.83203125" customWidth="1"/>
     <col min="7" max="7" width="21.6640625" customWidth="1"/>
   </cols>

</xml_diff>